<commit_message>
Update schema for: 	- showDateTime 	- displayTrueAs 	- displayFalseAs 	- displayAsProgress 	- displayAsLink
Update extraction for:
	- showDateTime
	- displayTrueAs
	- displayFalseAs
	- displayAsProgress
	- displayAsLink
</commit_message>
<xml_diff>
--- a/documents/TIF Function Detail.xlsx
+++ b/documents/TIF Function Detail.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
@@ -1487,7 +1487,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
@@ -1497,7 +1497,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>162</v>
       </c>
@@ -1511,29 +1511,29 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>158</v>
       </c>
       <c r="D6" s="12"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>159</v>
       </c>
       <c r="D7" s="13"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>160</v>
       </c>
@@ -1548,26 +1548,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="8" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="7" max="8" width="16.109375" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="13" width="21.42578125" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" customWidth="1"/>
+    <col min="11" max="11" width="18.88671875" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="21.44140625" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" customWidth="1"/>
+    <col min="15" max="15" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
@@ -1578,7 +1578,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>17</v>
       </c>
@@ -1610,7 +1610,7 @@
       <c r="Q3" s="9"/>
       <c r="R3" s="9"/>
     </row>
-    <row r="4" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -1632,7 +1632,7 @@
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
@@ -1672,7 +1672,7 @@
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>2</v>
       </c>
@@ -1720,7 +1720,7 @@
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>3</v>
       </c>
@@ -1768,7 +1768,7 @@
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>4</v>
       </c>
@@ -1808,7 +1808,7 @@
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
@@ -1846,7 +1846,7 @@
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>6</v>
       </c>
@@ -1868,7 +1868,7 @@
       <c r="G10" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="16" t="s">
         <v>166</v>
       </c>
       <c r="I10" s="16" t="s">
@@ -1890,7 +1890,7 @@
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>7</v>
       </c>
@@ -1921,7 +1921,7 @@
       <c r="J11" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="K11" s="22" t="s">
+      <c r="K11" s="16" t="s">
         <v>59</v>
       </c>
       <c r="L11" s="16" t="s">
@@ -1940,7 +1940,7 @@
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>8</v>
       </c>
@@ -1968,10 +1968,10 @@
       <c r="I12" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="J12" s="22" t="s">
+      <c r="J12" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="K12" s="22" t="s">
+      <c r="K12" s="16" t="s">
         <v>64</v>
       </c>
       <c r="L12" s="16" t="s">
@@ -1988,7 +1988,7 @@
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>9</v>
       </c>
@@ -2038,7 +2038,7 @@
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>10</v>
       </c>
@@ -2074,7 +2074,7 @@
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>73</v>
       </c>
@@ -2118,7 +2118,7 @@
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>11</v>
       </c>
@@ -2162,7 +2162,7 @@
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>12</v>
       </c>
@@ -2200,7 +2200,7 @@
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>13</v>
       </c>
@@ -2254,7 +2254,7 @@
       </c>
       <c r="R18" s="8"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>87</v>
       </c>
@@ -2300,7 +2300,7 @@
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>14</v>
       </c>
@@ -2334,7 +2334,7 @@
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>16</v>
       </c>
@@ -2396,7 +2396,7 @@
       <c r="Q24" s="9"/>
       <c r="R24" s="9"/>
     </row>
-    <row r="25" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>137</v>
       </c>
@@ -2428,7 +2428,7 @@
       <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>92</v>
       </c>
@@ -2484,7 +2484,7 @@
       <c r="Q30" s="9"/>
       <c r="R30" s="9"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>22</v>
       </c>
@@ -2514,7 +2514,7 @@
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>23</v>
       </c>
@@ -2540,7 +2540,7 @@
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>24</v>
       </c>
@@ -2570,7 +2570,7 @@
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>97</v>
       </c>
@@ -2594,7 +2594,7 @@
       <c r="Q34" s="8"/>
       <c r="R34" s="8"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>96</v>
       </c>
@@ -2618,7 +2618,7 @@
       <c r="Q35" s="8"/>
       <c r="R35" s="8"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>98</v>
       </c>
@@ -2642,7 +2642,7 @@
       <c r="Q36" s="8"/>
       <c r="R36" s="8"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>99</v>
       </c>
@@ -2674,7 +2674,7 @@
       <c r="Q37" s="8"/>
       <c r="R37" s="8"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>100</v>
       </c>
@@ -2714,7 +2714,7 @@
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>101</v>
       </c>
@@ -2738,7 +2738,7 @@
       <c r="Q39" s="8"/>
       <c r="R39" s="8"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>102</v>
       </c>
@@ -2762,7 +2762,7 @@
       <c r="Q40" s="8"/>
       <c r="R40" s="8"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>103</v>
       </c>
@@ -2794,7 +2794,7 @@
       <c r="Q41" s="8"/>
       <c r="R41" s="8"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
         <v>114</v>
       </c>
@@ -2832,7 +2832,7 @@
       <c r="Q42" s="8"/>
       <c r="R42" s="8"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>115</v>
       </c>
@@ -2864,7 +2864,7 @@
       <c r="Q43" s="8"/>
       <c r="R43" s="8"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
         <v>119</v>
       </c>
@@ -2892,7 +2892,7 @@
       <c r="Q44" s="8"/>
       <c r="R44" s="8"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>122</v>
       </c>
@@ -2926,7 +2926,7 @@
       <c r="Q45" s="8"/>
       <c r="R45" s="8"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
         <v>125</v>
       </c>
@@ -2974,7 +2974,7 @@
       <c r="Q46" s="8"/>
       <c r="R46" s="8"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
         <v>136</v>
       </c>
@@ -2998,7 +2998,7 @@
       <c r="Q47" s="8"/>
       <c r="R47" s="8"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -3018,7 +3018,7 @@
       <c r="Q48" s="8"/>
       <c r="R48" s="8"/>
     </row>
-    <row r="51" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A51" s="9" t="s">
         <v>28</v>
       </c>
@@ -3042,7 +3042,7 @@
       <c r="Q51" s="9"/>
       <c r="R51" s="9"/>
     </row>
-    <row r="52" spans="1:18" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
         <v>137</v>
       </c>
@@ -3072,7 +3072,7 @@
       <c r="Q52" s="11"/>
       <c r="R52" s="11"/>
     </row>
-    <row r="53" spans="1:18" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
         <v>92</v>
       </c>
@@ -3102,7 +3102,7 @@
       <c r="Q53" s="11"/>
       <c r="R53" s="11"/>
     </row>
-    <row r="55" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
         <v>29</v>
       </c>
@@ -3126,7 +3126,7 @@
       <c r="Q55" s="9"/>
       <c r="R55" s="9"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
         <v>137</v>
       </c>
@@ -3166,7 +3166,7 @@
       <c r="Q56" s="8"/>
       <c r="R56" s="8"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
         <v>92</v>
       </c>
@@ -3190,7 +3190,7 @@
       <c r="Q57" s="8"/>
       <c r="R57" s="8"/>
     </row>
-    <row r="60" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A60" s="9" t="s">
         <v>30</v>
       </c>
@@ -3214,7 +3214,7 @@
       <c r="Q60" s="9"/>
       <c r="R60" s="9"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
         <v>137</v>
       </c>
@@ -3252,7 +3252,7 @@
       <c r="Q61" s="8"/>
       <c r="R61" s="8"/>
     </row>
-    <row r="63" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A63" s="9" t="s">
         <v>31</v>
       </c>
@@ -3276,7 +3276,7 @@
       <c r="Q63" s="9"/>
       <c r="R63" s="9"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="8" t="s">
         <v>137</v>
       </c>
@@ -3312,7 +3312,7 @@
       <c r="Q64" s="8"/>
       <c r="R64" s="8"/>
     </row>
-    <row r="66" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A66" s="9" t="s">
         <v>19</v>
       </c>
@@ -3336,7 +3336,7 @@
       <c r="Q66" s="9"/>
       <c r="R66" s="9"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="8" t="s">
         <v>137</v>
       </c>
@@ -3374,7 +3374,7 @@
       <c r="Q67" s="8"/>
       <c r="R67" s="8"/>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="8"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
@@ -3394,7 +3394,7 @@
       <c r="Q68" s="8"/>
       <c r="R68" s="8"/>
     </row>
-    <row r="71" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A71" s="9" t="s">
         <v>20</v>
       </c>
@@ -3418,7 +3418,7 @@
       <c r="Q71" s="9"/>
       <c r="R71" s="9"/>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
         <v>137</v>
       </c>
@@ -3460,7 +3460,7 @@
       <c r="Q72" s="8"/>
       <c r="R72" s="8"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="8"/>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
@@ -3480,7 +3480,7 @@
       <c r="Q73" s="8"/>
       <c r="R73" s="8"/>
     </row>
-    <row r="78" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
         <v>21</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="82" spans="1:3" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
         <v>26</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="86" spans="1:3" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
         <v>27</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="90" spans="1:3" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A90" s="1" t="s">
         <v>32</v>
       </c>
@@ -3512,7 +3512,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="93" spans="1:3" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A93" s="1" t="s">
         <v>33</v>
       </c>
@@ -3535,22 +3535,22 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="13" width="21.42578125" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="7" max="8" width="16.109375" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="21.44140625" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" customWidth="1"/>
+    <col min="15" max="15" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
@@ -3561,7 +3561,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>17</v>
       </c>
@@ -3593,7 +3593,7 @@
       <c r="Q3" s="9"/>
       <c r="R3" s="9"/>
     </row>
-    <row r="4" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -3615,7 +3615,7 @@
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
@@ -3655,7 +3655,7 @@
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>2</v>
       </c>
@@ -3703,7 +3703,7 @@
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>3</v>
       </c>
@@ -3751,7 +3751,7 @@
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>4</v>
       </c>
@@ -3791,7 +3791,7 @@
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
@@ -3829,7 +3829,7 @@
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>6</v>
       </c>
@@ -3873,7 +3873,7 @@
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>7</v>
       </c>
@@ -3923,7 +3923,7 @@
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>8</v>
       </c>
@@ -3971,7 +3971,7 @@
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>9</v>
       </c>
@@ -4021,7 +4021,7 @@
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>10</v>
       </c>
@@ -4057,7 +4057,7 @@
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>73</v>
       </c>
@@ -4101,7 +4101,7 @@
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>11</v>
       </c>
@@ -4145,7 +4145,7 @@
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>12</v>
       </c>
@@ -4183,7 +4183,7 @@
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>13</v>
       </c>
@@ -4237,7 +4237,7 @@
       </c>
       <c r="R18" s="41"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>87</v>
       </c>
@@ -4283,7 +4283,7 @@
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>14</v>
       </c>
@@ -4317,7 +4317,7 @@
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>16</v>
       </c>
@@ -4379,7 +4379,7 @@
       <c r="Q24" s="9"/>
       <c r="R24" s="9"/>
     </row>
-    <row r="25" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>137</v>
       </c>
@@ -4411,7 +4411,7 @@
       <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>92</v>
       </c>
@@ -4443,7 +4443,7 @@
       <c r="Q26" s="8"/>
       <c r="R26" s="8"/>
     </row>
-    <row r="30" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>18</v>
       </c>
@@ -4467,7 +4467,7 @@
       <c r="Q30" s="9"/>
       <c r="R30" s="9"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>22</v>
       </c>
@@ -4497,7 +4497,7 @@
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>23</v>
       </c>
@@ -4523,7 +4523,7 @@
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>24</v>
       </c>
@@ -4553,7 +4553,7 @@
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>97</v>
       </c>
@@ -4577,7 +4577,7 @@
       <c r="Q34" s="8"/>
       <c r="R34" s="8"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>96</v>
       </c>
@@ -4601,7 +4601,7 @@
       <c r="Q35" s="8"/>
       <c r="R35" s="8"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>98</v>
       </c>
@@ -4625,7 +4625,7 @@
       <c r="Q36" s="8"/>
       <c r="R36" s="8"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>99</v>
       </c>
@@ -4657,7 +4657,7 @@
       <c r="Q37" s="8"/>
       <c r="R37" s="8"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>100</v>
       </c>
@@ -4697,7 +4697,7 @@
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>101</v>
       </c>
@@ -4721,7 +4721,7 @@
       <c r="Q39" s="8"/>
       <c r="R39" s="8"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>102</v>
       </c>
@@ -4745,7 +4745,7 @@
       <c r="Q40" s="8"/>
       <c r="R40" s="8"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>103</v>
       </c>
@@ -4777,7 +4777,7 @@
       <c r="Q41" s="8"/>
       <c r="R41" s="8"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
         <v>114</v>
       </c>
@@ -4815,7 +4815,7 @@
       <c r="Q42" s="8"/>
       <c r="R42" s="8"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>115</v>
       </c>
@@ -4847,7 +4847,7 @@
       <c r="Q43" s="8"/>
       <c r="R43" s="8"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
         <v>119</v>
       </c>
@@ -4875,7 +4875,7 @@
       <c r="Q44" s="8"/>
       <c r="R44" s="8"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>122</v>
       </c>
@@ -4909,7 +4909,7 @@
       <c r="Q45" s="8"/>
       <c r="R45" s="8"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
         <v>125</v>
       </c>
@@ -4957,7 +4957,7 @@
       <c r="Q46" s="8"/>
       <c r="R46" s="8"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
         <v>136</v>
       </c>
@@ -4981,7 +4981,7 @@
       <c r="Q47" s="8"/>
       <c r="R47" s="8"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -5001,20 +5001,20 @@
       <c r="Q48" s="8"/>
       <c r="R48" s="8"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="20" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="21" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="21"/>
     </row>
-    <row r="53" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A53" s="9" t="s">
         <v>28</v>
       </c>
@@ -5038,7 +5038,7 @@
       <c r="Q53" s="9"/>
       <c r="R53" s="9"/>
     </row>
-    <row r="54" spans="1:18" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
         <v>137</v>
       </c>
@@ -5068,7 +5068,7 @@
       <c r="Q54" s="11"/>
       <c r="R54" s="11"/>
     </row>
-    <row r="55" spans="1:18" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
         <v>92</v>
       </c>
@@ -5098,7 +5098,7 @@
       <c r="Q55" s="11"/>
       <c r="R55" s="11"/>
     </row>
-    <row r="57" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A57" s="9" t="s">
         <v>29</v>
       </c>
@@ -5122,7 +5122,7 @@
       <c r="Q57" s="9"/>
       <c r="R57" s="9"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
         <v>137</v>
       </c>
@@ -5162,7 +5162,7 @@
       <c r="Q58" s="8"/>
       <c r="R58" s="8"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
         <v>92</v>
       </c>
@@ -5202,10 +5202,10 @@
       <c r="Q59" s="8"/>
       <c r="R59" s="8"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H60" s="27"/>
     </row>
-    <row r="62" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A62" s="9" t="s">
         <v>30</v>
       </c>
@@ -5229,7 +5229,7 @@
       <c r="Q62" s="9"/>
       <c r="R62" s="9"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
         <v>137</v>
       </c>
@@ -5267,7 +5267,7 @@
       <c r="Q63" s="8"/>
       <c r="R63" s="8"/>
     </row>
-    <row r="65" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A65" s="9" t="s">
         <v>31</v>
       </c>
@@ -5291,7 +5291,7 @@
       <c r="Q65" s="9"/>
       <c r="R65" s="9"/>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
         <v>137</v>
       </c>
@@ -5325,7 +5325,7 @@
       <c r="Q66" s="8"/>
       <c r="R66" s="8"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
@@ -5345,7 +5345,7 @@
       <c r="Q67" s="8"/>
       <c r="R67" s="8"/>
     </row>
-    <row r="69" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A69" s="9" t="s">
         <v>19</v>
       </c>
@@ -5369,7 +5369,7 @@
       <c r="Q69" s="9"/>
       <c r="R69" s="9"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="8" t="s">
         <v>137</v>
       </c>
@@ -5405,7 +5405,7 @@
       <c r="Q70" s="8"/>
       <c r="R70" s="8"/>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
@@ -5425,7 +5425,7 @@
       <c r="Q71" s="8"/>
       <c r="R71" s="8"/>
     </row>
-    <row r="74" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A74" s="9" t="s">
         <v>20</v>
       </c>
@@ -5449,7 +5449,7 @@
       <c r="Q74" s="9"/>
       <c r="R74" s="9"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
         <v>15</v>
       </c>
@@ -5489,7 +5489,7 @@
       <c r="Q75" s="8"/>
       <c r="R75" s="8"/>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="8"/>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
@@ -5509,7 +5509,7 @@
       <c r="Q76" s="8"/>
       <c r="R76" s="8"/>
     </row>
-    <row r="81" spans="1:3" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
         <v>21</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="85" spans="1:3" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
         <v>26</v>
       </c>
@@ -5525,7 +5525,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="89" spans="1:3" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
         <v>27</v>
       </c>
@@ -5533,7 +5533,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="93" spans="1:3" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A93" s="1" t="s">
         <v>32</v>
       </c>
@@ -5541,7 +5541,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="96" spans="1:3" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A96" s="1" t="s">
         <v>33</v>
       </c>
@@ -5559,26 +5559,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="13" width="21.42578125" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="7" max="8" width="16.109375" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="21.44140625" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" customWidth="1"/>
+    <col min="15" max="15" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
@@ -5589,7 +5589,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>17</v>
       </c>
@@ -5621,7 +5621,7 @@
       <c r="Q3" s="9"/>
       <c r="R3" s="9"/>
     </row>
-    <row r="4" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -5643,7 +5643,7 @@
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
@@ -5683,7 +5683,7 @@
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>2</v>
       </c>
@@ -5731,7 +5731,7 @@
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>3</v>
       </c>
@@ -5779,7 +5779,7 @@
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>4</v>
       </c>
@@ -5819,7 +5819,7 @@
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
@@ -5857,7 +5857,7 @@
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>6</v>
       </c>
@@ -5879,7 +5879,7 @@
       <c r="G10" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="16" t="s">
         <v>166</v>
       </c>
       <c r="I10" s="16" t="s">
@@ -5901,7 +5901,7 @@
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>7</v>
       </c>
@@ -5932,7 +5932,7 @@
       <c r="J11" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="K11" s="22" t="s">
+      <c r="K11" s="16" t="s">
         <v>59</v>
       </c>
       <c r="L11" s="16" t="s">
@@ -5951,7 +5951,7 @@
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>8</v>
       </c>
@@ -5979,10 +5979,10 @@
       <c r="I12" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="J12" s="22" t="s">
+      <c r="J12" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="K12" s="22" t="s">
+      <c r="K12" s="16" t="s">
         <v>64</v>
       </c>
       <c r="L12" s="16" t="s">
@@ -5999,7 +5999,7 @@
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>9</v>
       </c>
@@ -6049,7 +6049,7 @@
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>10</v>
       </c>
@@ -6085,7 +6085,7 @@
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>73</v>
       </c>
@@ -6129,7 +6129,7 @@
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>11</v>
       </c>
@@ -6173,7 +6173,7 @@
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>12</v>
       </c>
@@ -6211,7 +6211,7 @@
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>13</v>
       </c>
@@ -6265,7 +6265,7 @@
       </c>
       <c r="R18" s="41"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>87</v>
       </c>
@@ -6311,7 +6311,7 @@
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>14</v>
       </c>
@@ -6345,7 +6345,7 @@
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>16</v>
       </c>
@@ -6407,7 +6407,7 @@
       <c r="Q24" s="9"/>
       <c r="R24" s="9"/>
     </row>
-    <row r="25" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>137</v>
       </c>
@@ -6437,7 +6437,7 @@
       <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -6481,7 +6481,7 @@
       <c r="Q30" s="9"/>
       <c r="R30" s="9"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>22</v>
       </c>
@@ -6511,7 +6511,7 @@
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>23</v>
       </c>
@@ -6537,7 +6537,7 @@
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>24</v>
       </c>
@@ -6567,7 +6567,7 @@
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>97</v>
       </c>
@@ -6591,7 +6591,7 @@
       <c r="Q34" s="8"/>
       <c r="R34" s="8"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>96</v>
       </c>
@@ -6615,7 +6615,7 @@
       <c r="Q35" s="8"/>
       <c r="R35" s="8"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>98</v>
       </c>
@@ -6639,7 +6639,7 @@
       <c r="Q36" s="8"/>
       <c r="R36" s="8"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>99</v>
       </c>
@@ -6671,7 +6671,7 @@
       <c r="Q37" s="8"/>
       <c r="R37" s="8"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>100</v>
       </c>
@@ -6711,7 +6711,7 @@
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>101</v>
       </c>
@@ -6735,7 +6735,7 @@
       <c r="Q39" s="8"/>
       <c r="R39" s="8"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>102</v>
       </c>
@@ -6759,7 +6759,7 @@
       <c r="Q40" s="8"/>
       <c r="R40" s="8"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>103</v>
       </c>
@@ -6791,7 +6791,7 @@
       <c r="Q41" s="8"/>
       <c r="R41" s="8"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>114</v>
       </c>
@@ -6829,7 +6829,7 @@
       <c r="Q42" s="8"/>
       <c r="R42" s="8"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>115</v>
       </c>
@@ -6861,7 +6861,7 @@
       <c r="Q43" s="8"/>
       <c r="R43" s="8"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>119</v>
       </c>
@@ -6889,7 +6889,7 @@
       <c r="Q44" s="8"/>
       <c r="R44" s="8"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>122</v>
       </c>
@@ -6919,7 +6919,7 @@
       <c r="Q45" s="8"/>
       <c r="R45" s="8"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>125</v>
       </c>
@@ -6967,7 +6967,7 @@
       <c r="Q46" s="8"/>
       <c r="R46" s="8"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>136</v>
       </c>
@@ -6991,7 +6991,7 @@
       <c r="Q47" s="8"/>
       <c r="R47" s="8"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -7107,7 +7107,7 @@
       <c r="Q55" s="9"/>
       <c r="R55" s="9"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>137</v>
       </c>
@@ -7145,7 +7145,7 @@
       <c r="Q56" s="8"/>
       <c r="R56" s="8"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -7189,7 +7189,7 @@
       <c r="Q60" s="9"/>
       <c r="R60" s="9"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>137</v>
       </c>
@@ -7225,7 +7225,7 @@
       <c r="Q61" s="8"/>
       <c r="R61" s="8"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="E62" s="27"/>
     </row>
     <row r="63" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
@@ -7252,7 +7252,7 @@
       <c r="Q63" s="9"/>
       <c r="R63" s="9"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>137</v>
       </c>
@@ -7282,7 +7282,7 @@
       <c r="Q64" s="8"/>
       <c r="R64" s="8"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>92</v>
       </c>
@@ -7328,7 +7328,7 @@
       <c r="Q67" s="9"/>
       <c r="R67" s="9"/>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>137</v>
       </c>
@@ -7364,7 +7364,7 @@
       <c r="Q68" s="8"/>
       <c r="R68" s="8"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
@@ -7408,7 +7408,7 @@
       <c r="Q72" s="9"/>
       <c r="R72" s="9"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
         <v>15</v>
       </c>
@@ -7448,7 +7448,7 @@
       <c r="Q73" s="8"/>
       <c r="R73" s="8"/>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
@@ -7476,7 +7476,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="83" spans="1:2" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
         <v>26</v>
       </c>
@@ -7484,7 +7484,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="87" spans="1:2" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
         <v>27</v>
       </c>
@@ -7492,12 +7492,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="91" spans="1:2" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A91" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="94" spans="1:2" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
         <v>33</v>
       </c>
@@ -7517,12 +7517,12 @@
       <selection activeCell="A17" sqref="A17:F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="33"/>
-    <col min="2" max="3" width="9.140625" style="34"/>
-    <col min="4" max="4" width="55.7109375" style="30" customWidth="1"/>
-    <col min="5" max="5" width="57.7109375" style="30" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="33"/>
+    <col min="2" max="3" width="9.109375" style="34"/>
+    <col min="4" max="4" width="55.6640625" style="30" customWidth="1"/>
+    <col min="5" max="5" width="57.6640625" style="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -7545,7 +7545,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>185</v>
       </c>
@@ -7583,7 +7583,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>196</v>
       </c>
@@ -7615,7 +7615,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>200</v>
       </c>
@@ -7633,7 +7633,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>202</v>
       </c>
@@ -7665,7 +7665,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
         <v>206</v>
       </c>
@@ -7699,7 +7699,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>210</v>
       </c>
@@ -7751,7 +7751,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
         <v>217</v>
       </c>
@@ -7769,7 +7769,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
         <v>219</v>
       </c>
@@ -7783,7 +7783,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>221</v>
       </c>
@@ -7801,7 +7801,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
         <v>223</v>
       </c>
@@ -7826,15 +7826,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="30" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="30" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" style="30" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" style="30" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="30" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" style="30" customWidth="1"/>
     <col min="4" max="4" width="21" style="30" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7848,7 +7848,7 @@
       </c>
       <c r="D1" s="34"/>
     </row>
-    <row r="3" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
         <v>53</v>
       </c>
@@ -7862,7 +7862,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="s">
         <v>229</v>
       </c>
@@ -7874,7 +7874,7 @@
       </c>
       <c r="D4" s="44"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="44"/>
       <c r="B5" s="44" t="s">
         <v>43</v>
@@ -7884,7 +7884,7 @@
       </c>
       <c r="D5" s="44"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="44"/>
       <c r="B6" s="44" t="s">
         <v>42</v>
@@ -7894,19 +7894,19 @@
       </c>
       <c r="D6" s="44"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="44"/>
       <c r="B7" s="44"/>
       <c r="C7" s="44"/>
       <c r="D7" s="44"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="44"/>
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
       <c r="D8" s="44"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="s">
         <v>13</v>
       </c>
@@ -7916,7 +7916,7 @@
       <c r="C9" s="44"/>
       <c r="D9" s="44"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="44"/>
       <c r="B10" s="44" t="s">
         <v>80</v>
@@ -7924,7 +7924,7 @@
       <c r="C10" s="44"/>
       <c r="D10" s="44"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="44"/>
       <c r="B11" s="44" t="s">
         <v>82</v>
@@ -7932,19 +7932,19 @@
       <c r="C11" s="44"/>
       <c r="D11" s="44"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="44"/>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
       <c r="D12" s="44"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="44"/>
       <c r="B13" s="44"/>
       <c r="C13" s="44"/>
       <c r="D13" s="44"/>
     </row>
-    <row r="17" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="45" t="s">
         <v>15</v>
       </c>
@@ -7958,7 +7958,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="44"/>
       <c r="B18" s="44" t="s">
         <v>125</v>
@@ -7968,7 +7968,7 @@
       </c>
       <c r="D18" s="44"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="44"/>
       <c r="B19" s="44" t="s">
         <v>122</v>
@@ -7978,7 +7978,7 @@
       </c>
       <c r="D19" s="44"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="44"/>
       <c r="B20" s="44" t="s">
         <v>114</v>
@@ -7988,7 +7988,7 @@
       </c>
       <c r="D20" s="44"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="44"/>
       <c r="B21" s="44" t="s">
         <v>103</v>
@@ -8008,7 +8008,7 @@
       </c>
       <c r="D22" s="44"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="44"/>
       <c r="B23" s="44" t="s">
         <v>115</v>
@@ -8028,7 +8028,7 @@
       </c>
       <c r="D24" s="44"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="44"/>
       <c r="B25" s="44" t="s">
         <v>234</v>
@@ -8036,13 +8036,13 @@
       <c r="C25" s="44"/>
       <c r="D25" s="44"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="44"/>
       <c r="B26" s="44"/>
       <c r="C26" s="44"/>
       <c r="D26" s="44"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="44"/>
       <c r="B27" s="44"/>
       <c r="C27" s="44"/>

</xml_diff>

<commit_message>
Adding "DisplayAs" in schema / field reader / documentation New "DisplayAsType" simple type in schema for managing Checkbox / DropDown value.
</commit_message>
<xml_diff>
--- a/documents/TIF Function Detail.xlsx
+++ b/documents/TIF Function Detail.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
@@ -1548,8 +1548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1965,7 +1965,7 @@
       <c r="H12" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="I12" s="16" t="s">
         <v>62</v>
       </c>
       <c r="J12" s="16" t="s">
@@ -2460,7 +2460,7 @@
       <c r="Q26" s="8"/>
       <c r="R26" s="8"/>
     </row>
-    <row r="30" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>18</v>
       </c>
@@ -2484,7 +2484,7 @@
       <c r="Q30" s="9"/>
       <c r="R30" s="9"/>
     </row>
-    <row r="31" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>22</v>
       </c>
@@ -2514,7 +2514,7 @@
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
     </row>
-    <row r="32" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>23</v>
       </c>
@@ -2540,7 +2540,7 @@
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
     </row>
-    <row r="33" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>24</v>
       </c>
@@ -2570,7 +2570,7 @@
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
     </row>
-    <row r="34" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>97</v>
       </c>
@@ -2594,7 +2594,7 @@
       <c r="Q34" s="8"/>
       <c r="R34" s="8"/>
     </row>
-    <row r="35" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>96</v>
       </c>
@@ -2618,7 +2618,7 @@
       <c r="Q35" s="8"/>
       <c r="R35" s="8"/>
     </row>
-    <row r="36" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>98</v>
       </c>
@@ -5559,8 +5559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5976,7 +5976,7 @@
       <c r="H12" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="I12" s="16" t="s">
         <v>62</v>
       </c>
       <c r="J12" s="16" t="s">
@@ -6511,7 +6511,7 @@
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
     </row>
-    <row r="32" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>23</v>
       </c>
@@ -6537,7 +6537,7 @@
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
     </row>
-    <row r="33" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>24</v>
       </c>
@@ -6567,7 +6567,7 @@
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
     </row>
-    <row r="34" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>97</v>
       </c>
@@ -6591,7 +6591,7 @@
       <c r="Q34" s="8"/>
       <c r="R34" s="8"/>
     </row>
-    <row r="35" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>96</v>
       </c>
@@ -6615,7 +6615,7 @@
       <c r="Q35" s="8"/>
       <c r="R35" s="8"/>
     </row>
-    <row r="36" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>98</v>
       </c>
@@ -6639,7 +6639,7 @@
       <c r="Q36" s="8"/>
       <c r="R36" s="8"/>
     </row>
-    <row r="37" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>99</v>
       </c>
@@ -6671,7 +6671,7 @@
       <c r="Q37" s="8"/>
       <c r="R37" s="8"/>
     </row>
-    <row r="38" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>100</v>
       </c>
@@ -6711,7 +6711,7 @@
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
     </row>
-    <row r="39" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>101</v>
       </c>
@@ -6735,7 +6735,7 @@
       <c r="Q39" s="8"/>
       <c r="R39" s="8"/>
     </row>
-    <row r="40" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>102</v>
       </c>
@@ -6759,7 +6759,7 @@
       <c r="Q40" s="8"/>
       <c r="R40" s="8"/>
     </row>
-    <row r="41" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>103</v>
       </c>
@@ -6791,7 +6791,7 @@
       <c r="Q41" s="8"/>
       <c r="R41" s="8"/>
     </row>
-    <row r="42" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
         <v>114</v>
       </c>
@@ -6829,7 +6829,7 @@
       <c r="Q42" s="8"/>
       <c r="R42" s="8"/>
     </row>
-    <row r="43" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>115</v>
       </c>
@@ -6861,7 +6861,7 @@
       <c r="Q43" s="8"/>
       <c r="R43" s="8"/>
     </row>
-    <row r="44" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
         <v>119</v>
       </c>
@@ -6889,7 +6889,7 @@
       <c r="Q44" s="8"/>
       <c r="R44" s="8"/>
     </row>
-    <row r="45" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>122</v>
       </c>
@@ -6919,7 +6919,7 @@
       <c r="Q45" s="8"/>
       <c r="R45" s="8"/>
     </row>
-    <row r="46" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
         <v>125</v>
       </c>
@@ -6967,7 +6967,7 @@
       <c r="Q46" s="8"/>
       <c r="R46" s="8"/>
     </row>
-    <row r="47" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
         <v>136</v>
       </c>
@@ -6991,7 +6991,7 @@
       <c r="Q47" s="8"/>
       <c r="R47" s="8"/>
     </row>
-    <row r="48" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -7011,7 +7011,7 @@
       <c r="Q48" s="8"/>
       <c r="R48" s="8"/>
     </row>
-    <row r="51" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A51" s="9" t="s">
         <v>28</v>
       </c>
@@ -7035,7 +7035,7 @@
       <c r="Q51" s="9"/>
       <c r="R51" s="9"/>
     </row>
-    <row r="52" spans="1:18" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
         <v>137</v>
       </c>
@@ -7063,7 +7063,7 @@
       <c r="Q52" s="11"/>
       <c r="R52" s="11"/>
     </row>
-    <row r="53" spans="1:18" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="11"/>
       <c r="B53" s="11"/>
       <c r="C53" s="11"/>
@@ -7083,7 +7083,7 @@
       <c r="Q53" s="11"/>
       <c r="R53" s="11"/>
     </row>
-    <row r="55" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
         <v>29</v>
       </c>
@@ -7107,7 +7107,7 @@
       <c r="Q55" s="9"/>
       <c r="R55" s="9"/>
     </row>
-    <row r="56" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
         <v>137</v>
       </c>
@@ -7145,7 +7145,7 @@
       <c r="Q56" s="8"/>
       <c r="R56" s="8"/>
     </row>
-    <row r="57" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -7165,7 +7165,7 @@
       <c r="Q57" s="8"/>
       <c r="R57" s="8"/>
     </row>
-    <row r="60" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A60" s="9" t="s">
         <v>30</v>
       </c>
@@ -7189,7 +7189,7 @@
       <c r="Q60" s="9"/>
       <c r="R60" s="9"/>
     </row>
-    <row r="61" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
         <v>137</v>
       </c>
@@ -7225,10 +7225,10 @@
       <c r="Q61" s="8"/>
       <c r="R61" s="8"/>
     </row>
-    <row r="62" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="E62" s="27"/>
     </row>
-    <row r="63" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A63" s="9" t="s">
         <v>31</v>
       </c>
@@ -7252,7 +7252,7 @@
       <c r="Q63" s="9"/>
       <c r="R63" s="9"/>
     </row>
-    <row r="64" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="8" t="s">
         <v>137</v>
       </c>
@@ -7282,7 +7282,7 @@
       <c r="Q64" s="8"/>
       <c r="R64" s="8"/>
     </row>
-    <row r="65" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
         <v>92</v>
       </c>
@@ -7304,7 +7304,7 @@
       <c r="Q65" s="8"/>
       <c r="R65" s="8"/>
     </row>
-    <row r="67" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A67" s="9" t="s">
         <v>19</v>
       </c>
@@ -7328,7 +7328,7 @@
       <c r="Q67" s="9"/>
       <c r="R67" s="9"/>
     </row>
-    <row r="68" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="8" t="s">
         <v>137</v>
       </c>
@@ -7364,7 +7364,7 @@
       <c r="Q68" s="8"/>
       <c r="R68" s="8"/>
     </row>
-    <row r="69" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
@@ -7384,7 +7384,7 @@
       <c r="Q69" s="8"/>
       <c r="R69" s="8"/>
     </row>
-    <row r="72" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A72" s="9" t="s">
         <v>20</v>
       </c>
@@ -7408,7 +7408,7 @@
       <c r="Q72" s="9"/>
       <c r="R72" s="9"/>
     </row>
-    <row r="73" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
         <v>15</v>
       </c>
@@ -7448,7 +7448,7 @@
       <c r="Q73" s="8"/>
       <c r="R73" s="8"/>
     </row>
-    <row r="74" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
@@ -7468,7 +7468,7 @@
       <c r="Q74" s="8"/>
       <c r="R74" s="8"/>
     </row>
-    <row r="79" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
         <v>21</v>
       </c>
@@ -7504,7 +7504,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added cycleDetection / showVariableHeighRows in schema. Added cycleDetection / showVariableHeighRows / displayStyle extraction in FieldReader Updated TIF Function Details accordingly.
</commit_message>
<xml_diff>
--- a/documents/TIF Function Detail.xlsx
+++ b/documents/TIF Function Detail.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
@@ -1483,8 +1483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1548,8 +1548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1564,10 +1564,11 @@
     <col min="9" max="9" width="17" customWidth="1"/>
     <col min="10" max="10" width="15.44140625" customWidth="1"/>
     <col min="11" max="11" width="18.88671875" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="12" max="12" width="22.5546875" customWidth="1"/>
     <col min="13" max="13" width="21.44140625" customWidth="1"/>
     <col min="14" max="14" width="16.44140625" customWidth="1"/>
     <col min="15" max="15" width="16.109375" customWidth="1"/>
+    <col min="16" max="16" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
@@ -1694,7 +1695,7 @@
       <c r="G6" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="16" t="s">
         <v>45</v>
       </c>
       <c r="I6" s="16" t="s">
@@ -2152,7 +2153,7 @@
       <c r="K16" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="L16" s="22" t="s">
+      <c r="L16" s="16" t="s">
         <v>77</v>
       </c>
       <c r="M16" s="8"/>
@@ -2234,7 +2235,7 @@
       <c r="K18" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="L18" s="22" t="s">
+      <c r="L18" s="16" t="s">
         <v>81</v>
       </c>
       <c r="M18" s="16" t="s">
@@ -2246,7 +2247,7 @@
       <c r="O18" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="P18" s="22" t="s">
+      <c r="P18" s="16" t="s">
         <v>83</v>
       </c>
       <c r="Q18" s="22" t="s">
@@ -3531,7 +3532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -5560,7 +5561,7 @@
   <dimension ref="A1:R94"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A18" sqref="A18:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5578,7 +5579,7 @@
     <col min="12" max="12" width="15.33203125" customWidth="1"/>
     <col min="13" max="13" width="21.44140625" customWidth="1"/>
     <col min="14" max="14" width="16.44140625" customWidth="1"/>
-    <col min="15" max="15" width="16.109375" customWidth="1"/>
+    <col min="15" max="15" width="40.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
@@ -5705,7 +5706,7 @@
       <c r="G6" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="16" t="s">
         <v>45</v>
       </c>
       <c r="I6" s="16" t="s">
@@ -6157,13 +6158,13 @@
       <c r="I16" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="J16" s="22" t="s">
+      <c r="J16" s="16" t="s">
         <v>76</v>
       </c>
       <c r="K16" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="L16" s="22" t="s">
+      <c r="L16" s="16" t="s">
         <v>77</v>
       </c>
       <c r="M16" s="8"/>
@@ -6236,7 +6237,7 @@
       <c r="H18" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="I18" s="22" t="s">
+      <c r="I18" s="16" t="s">
         <v>76</v>
       </c>
       <c r="J18" s="16" t="s">
@@ -6245,7 +6246,7 @@
       <c r="K18" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="L18" s="22" t="s">
+      <c r="L18" s="16" t="s">
         <v>81</v>
       </c>
       <c r="M18" s="16" t="s">
@@ -6257,7 +6258,7 @@
       <c r="O18" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="P18" s="22" t="s">
+      <c r="P18" s="16" t="s">
         <v>83</v>
       </c>
       <c r="Q18" s="22" t="s">

</xml_diff>

<commit_message>
Added suggestions/suggestion, paramSubstitution, and storeToHistoryFrequency in schema for Field. Added suggestions/suggestion, paramSubstitution, and storeToHistoryFrequency in schema for Field Reader. Updated TIF Function Detail document accordingly
</commit_message>
<xml_diff>
--- a/documents/TIF Function Detail.xlsx
+++ b/documents/TIF Function Detail.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
@@ -1483,7 +1483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -1548,8 +1548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2283,10 +2283,10 @@
       <c r="I19" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="J19" s="22" t="s">
+      <c r="J19" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="K19" s="22" t="s">
+      <c r="K19" s="16" t="s">
         <v>69</v>
       </c>
       <c r="L19" s="16" t="s">
@@ -3532,7 +3532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -5560,8 +5560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6294,16 +6294,16 @@
       <c r="I19" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="J19" s="22" t="s">
+      <c r="J19" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="K19" s="22" t="s">
+      <c r="K19" s="16" t="s">
         <v>69</v>
       </c>
       <c r="L19" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="M19" s="22" t="s">
+      <c r="M19" s="16" t="s">
         <v>89</v>
       </c>
       <c r="N19" s="8"/>

</xml_diff>

<commit_message>
Update param substitutions in TIF Function Detail and fix the substituteParameter attribute setting in FieldReader.
</commit_message>
<xml_diff>
--- a/documents/TIF Function Detail.xlsx
+++ b/documents/TIF Function Detail.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
@@ -1548,8 +1548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2029,7 +2029,7 @@
       <c r="M13" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="N13" s="22" t="s">
+      <c r="N13" s="16" t="s">
         <v>69</v>
       </c>
       <c r="O13" s="16" t="s">
@@ -2061,7 +2061,7 @@
       <c r="G14" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="22" t="s">
+      <c r="H14" s="16" t="s">
         <v>71</v>
       </c>
       <c r="I14" s="8"/>
@@ -2373,7 +2373,7 @@
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
     </row>
-    <row r="24" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A24" s="9" t="s">
         <v>34</v>
       </c>
@@ -2397,7 +2397,7 @@
       <c r="Q24" s="9"/>
       <c r="R24" s="9"/>
     </row>
-    <row r="25" spans="1:18" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>137</v>
       </c>
@@ -2429,7 +2429,7 @@
       <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
     </row>
-    <row r="26" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>92</v>
       </c>
@@ -5560,8 +5560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H14" sqref="A14:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6040,7 +6040,7 @@
       <c r="M13" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="N13" s="22" t="s">
+      <c r="N13" s="16" t="s">
         <v>69</v>
       </c>
       <c r="O13" s="22" t="s">
@@ -6408,7 +6408,7 @@
       <c r="Q24" s="9"/>
       <c r="R24" s="9"/>
     </row>
-    <row r="25" spans="1:18" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>137</v>
       </c>
@@ -6438,7 +6438,7 @@
       <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
     </row>
-    <row r="26" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -6458,7 +6458,7 @@
       <c r="Q26" s="8"/>
       <c r="R26" s="8"/>
     </row>
-    <row r="30" spans="1:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>18</v>
       </c>
@@ -6482,7 +6482,7 @@
       <c r="Q30" s="9"/>
       <c r="R30" s="9"/>
     </row>
-    <row r="31" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>22</v>
       </c>
@@ -8019,7 +8019,7 @@
       </c>
       <c r="D23" s="44"/>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="44"/>
       <c r="B24" s="44" t="s">
         <v>24</v>
@@ -8029,7 +8029,7 @@
       </c>
       <c r="D24" s="44"/>
     </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="44"/>
       <c r="B25" s="44" t="s">
         <v>234</v>
@@ -8037,13 +8037,13 @@
       <c r="C25" s="44"/>
       <c r="D25" s="44"/>
     </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="44"/>
       <c r="B26" s="44"/>
       <c r="C26" s="44"/>
       <c r="D26" s="44"/>
     </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="44"/>
       <c r="B27" s="44"/>
       <c r="C27" s="44"/>

</xml_diff>

<commit_message>
Added ReportsDefinition / ReportDefinition in schema Added report reading (name / description / .query / sharing / isAdmin / Recipe Parameters) Updated TIF Function Detail document accordingly
</commit_message>
<xml_diff>
--- a/documents/TIF Function Detail.xlsx
+++ b/documents/TIF Function Detail.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
@@ -98,6 +98,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="G79" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Shall we transfert only admin reports ?</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -181,12 +205,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="G80" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Shall we transfert only admin reports ?</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="245">
   <si>
     <t>Fields</t>
   </si>
@@ -915,13 +963,19 @@
   </si>
   <si>
     <t>Objects are keyed on their name (not display name)</t>
+  </si>
+  <si>
+    <t>is Admin</t>
+  </si>
+  <si>
+    <t>Recipe Parameters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -997,6 +1051,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1483,8 +1550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1502,7 +1569,7 @@
         <v>162</v>
       </c>
       <c r="B2" s="15">
-        <v>41551</v>
+        <v>41552</v>
       </c>
       <c r="E2" t="s">
         <v>176</v>
@@ -1548,8 +1615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:F27"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3482,11 +3549,56 @@
       <c r="R73" s="8"/>
     </row>
     <row r="78" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>151</v>
+      <c r="B78" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="9"/>
+      <c r="J78" s="9"/>
+      <c r="K78" s="9"/>
+      <c r="L78" s="9"/>
+      <c r="M78" s="9"/>
+      <c r="N78" s="9"/>
+      <c r="O78" s="9"/>
+      <c r="P78" s="9"/>
+      <c r="Q78" s="9"/>
+      <c r="R78" s="9"/>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A79" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C79" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="D79" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E79" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F79" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="G79" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="H79" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="I79" s="16" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="82" spans="1:3" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
@@ -3523,7 +3635,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -3532,7 +3644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -5560,8 +5672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H14" sqref="A14:H14"/>
+    <sheetView topLeftCell="A61" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5572,7 +5684,8 @@
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="15.109375" customWidth="1"/>
-    <col min="7" max="8" width="16.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" customWidth="1"/>
     <col min="9" max="9" width="15.44140625" customWidth="1"/>
     <col min="10" max="10" width="13.5546875" customWidth="1"/>
     <col min="11" max="11" width="13.88671875" customWidth="1"/>
@@ -7470,11 +7583,56 @@
       <c r="R74" s="8"/>
     </row>
     <row r="79" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>151</v>
+      <c r="B79" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
+      <c r="I79" s="9"/>
+      <c r="J79" s="9"/>
+      <c r="K79" s="9"/>
+      <c r="L79" s="9"/>
+      <c r="M79" s="9"/>
+      <c r="N79" s="9"/>
+      <c r="O79" s="9"/>
+      <c r="P79" s="9"/>
+      <c r="Q79" s="9"/>
+      <c r="R79" s="9"/>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A80" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C80" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="D80" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E80" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F80" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="G80" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="H80" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="I80" s="16" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="83" spans="1:2" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Updated script-gen for report deployment using recipeParams instead of report file. Updated TIF Function Detail accordingly. Comited Report def in schema.
</commit_message>
<xml_diff>
--- a/documents/TIF Function Detail.xlsx
+++ b/documents/TIF Function Detail.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956"/>
+    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
@@ -132,6 +132,40 @@
     <author>Author</author>
   </authors>
   <commentList>
+    <comment ref="G82" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Shall we transfert only admin reports ?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
     <comment ref="N13" authorId="0">
       <text>
         <r>
@@ -234,7 +268,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="245">
   <si>
     <t>Fields</t>
   </si>
@@ -1550,7 +1584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -1616,7 +1650,7 @@
   <dimension ref="A1:R93"/>
   <sheetViews>
     <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+      <selection activeCell="A78" sqref="A78:XFD79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3641,11 +3675,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5622,15 +5656,60 @@
       <c r="Q76" s="8"/>
       <c r="R76" s="8"/>
     </row>
-    <row r="81" spans="1:3" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A81" s="1" t="s">
+    <row r="81" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A81" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="9"/>
+      <c r="I81" s="9"/>
+      <c r="J81" s="9"/>
+      <c r="K81" s="9"/>
+      <c r="L81" s="9"/>
+      <c r="M81" s="9"/>
+      <c r="N81" s="9"/>
+      <c r="O81" s="9"/>
+      <c r="P81" s="9"/>
+      <c r="Q81" s="9"/>
+      <c r="R81" s="9"/>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A82" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B82" s="8" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="C82" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="D82" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E82" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F82" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="G82" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="H82" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="I82" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
         <v>26</v>
       </c>
@@ -5638,7 +5717,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="89" spans="1:3" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
         <v>27</v>
       </c>
@@ -5646,7 +5725,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="93" spans="1:3" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A93" s="1" t="s">
         <v>32</v>
       </c>
@@ -5654,7 +5733,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="96" spans="1:3" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:18" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A96" s="1" t="s">
         <v>33</v>
       </c>
@@ -5665,6 +5744,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5672,8 +5752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H21" sqref="A14:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7985,8 +8065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A24" sqref="A22:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8033,7 +8113,7 @@
       </c>
       <c r="D4" s="44"/>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="44"/>
       <c r="B5" s="44" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Added in script gen: 	Group : multivalued 	IBPL : display as link 	Logical: display true as, display false as, display as 	LongText : substitute params, text index 	QBR : display style, display rows, show variable height 	Relationship: show variable height, display style, cycle detection 	Shorttext: substitute parameters
Deleted duplicated entries in schema (subsParams & showTallRows)

Updated TIF Function Detail document accordingly
</commit_message>
<xml_diff>
--- a/documents/TIF Function Detail.xlsx
+++ b/documents/TIF Function Detail.xlsx
@@ -1649,8 +1649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78:XFD79"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3678,8 +3678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3694,7 +3694,7 @@
     <col min="9" max="9" width="15.5546875" customWidth="1"/>
     <col min="10" max="10" width="13.5546875" customWidth="1"/>
     <col min="11" max="11" width="13.88671875" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="12" max="12" width="36" customWidth="1"/>
     <col min="13" max="13" width="21.44140625" customWidth="1"/>
     <col min="14" max="14" width="16.44140625" customWidth="1"/>
     <col min="15" max="15" width="16.109375" customWidth="1"/>
@@ -3960,7 +3960,7 @@
       <c r="G9" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="16" t="s">
         <v>55</v>
       </c>
       <c r="I9" s="16" t="s">
@@ -3998,7 +3998,7 @@
       <c r="G10" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="16" t="s">
         <v>166</v>
       </c>
       <c r="I10" s="16" t="s">
@@ -4020,7 +4020,7 @@
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
     </row>
-    <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>7</v>
       </c>
@@ -4095,13 +4095,13 @@
       <c r="H12" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="I12" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="J12" s="22" t="s">
+      <c r="J12" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="K12" s="22" t="s">
+      <c r="K12" s="16" t="s">
         <v>64</v>
       </c>
       <c r="L12" s="16" t="s">
@@ -4158,10 +4158,10 @@
       <c r="M13" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="N13" s="22" t="s">
+      <c r="N13" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="O13" s="22" t="s">
+      <c r="O13" s="16" t="s">
         <v>70</v>
       </c>
       <c r="P13" s="8"/>
@@ -4276,13 +4276,13 @@
       <c r="I16" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="J16" s="22" t="s">
+      <c r="J16" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="K16" s="22" t="s">
+      <c r="K16" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="L16" s="22" t="s">
+      <c r="L16" s="16" t="s">
         <v>77</v>
       </c>
       <c r="M16" s="8"/>
@@ -5752,8 +5752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H21" sqref="A14:H21"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>